<commit_message>
fixes of local search
</commit_message>
<xml_diff>
--- a/schedule_local.xlsx
+++ b/schedule_local.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
   <si>
     <t>09:00 - 09:30</t>
   </si>
@@ -100,85 +100,85 @@
     <t>407</t>
   </si>
   <si>
+    <t>Petroleum Geophysics</t>
+  </si>
+  <si>
+    <t>Introduction to Power Systems</t>
+  </si>
+  <si>
+    <t>Numerical Methods for Partial Differential Equations</t>
+  </si>
+  <si>
+    <t>Stem Cells</t>
+  </si>
+  <si>
+    <t>Intellectual Property and Technological Innovation</t>
+  </si>
+  <si>
+    <t>Thermal Fluid Sciences</t>
+  </si>
+  <si>
+    <t>Quantum Fluids</t>
+  </si>
+  <si>
+    <t>Bioinformatics Lab Course 2</t>
+  </si>
+  <si>
+    <t>Introduction Device Physics</t>
+  </si>
+  <si>
+    <t>RNA Biology</t>
+  </si>
+  <si>
+    <t>Feb 2, 9, 16, March 1</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Materials Chemistry</t>
+  </si>
+  <si>
+    <t>Mathematical Methods of Optical Communication</t>
+  </si>
+  <si>
+    <t>Introduction to Composite Materials and Structures</t>
+  </si>
+  <si>
+    <t>Bayesian Methods - Adv Machine Learning</t>
+  </si>
+  <si>
+    <t>Feb 3, 10, 17, 24, March 2, 9</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Advanced Molecular Biology Techniques 1</t>
+  </si>
+  <si>
+    <t>Feb 4, 11, 18, 25, March 3, 10</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Dynamic Systems and Control</t>
+  </si>
+  <si>
+    <t>Space Sector Course</t>
+  </si>
+  <si>
+    <t>Feb 5, 12, 19, 26, March 4, 11</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
     <t>408</t>
   </si>
   <si>
-    <t>Mathematical Methods of Optical Communication</t>
-  </si>
-  <si>
-    <t>Introduction to Power Systems</t>
-  </si>
-  <si>
-    <t>Numerical Methods for Partial Differential Equations</t>
-  </si>
-  <si>
-    <t>Stem Cells</t>
-  </si>
-  <si>
-    <t>Dynamic Systems and Control</t>
-  </si>
-  <si>
-    <t>Thermal Fluid Sciences</t>
-  </si>
-  <si>
-    <t>Materials Chemistry</t>
-  </si>
-  <si>
-    <t>Quantum Fluids</t>
-  </si>
-  <si>
-    <t>RNA Biology</t>
-  </si>
-  <si>
-    <t>Introduction Device Physics</t>
-  </si>
-  <si>
-    <t>Bioinformatics Lab Course 2</t>
-  </si>
-  <si>
-    <t>Space Sector Course</t>
-  </si>
-  <si>
-    <t>Feb 2, 9, 16, March 1</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Petroleum Geophysics</t>
-  </si>
-  <si>
-    <t>Introduction to Composite Materials and Structures</t>
-  </si>
-  <si>
-    <t>Bayesian Methods - Adv Machine Learning</t>
-  </si>
-  <si>
-    <t>Intellectual Property and Technological Innovation</t>
-  </si>
-  <si>
-    <t>Feb 3, 10, 17, 24, March 2, 9</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Advanced Molecular Biology Techniques 1</t>
-  </si>
-  <si>
-    <t>Feb 4, 11, 18, 25, March 3, 10</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Quantum Fluids(Energy)</t>
-  </si>
-  <si>
-    <t>Feb 5, 12, 19, 26, March 4, 11</t>
-  </si>
-  <si>
-    <t>Friday</t>
+    <t>Mathematical Methods of Optical Communication(Energy)</t>
   </si>
   <si>
     <t>WEEK 1-6</t>
@@ -255,85 +255,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEDF279"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD379F2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7988F2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFACF279"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF79F2D8"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2B579"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9179F2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF83F279"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF79F2B0"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF28C79"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF279A7"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF79CAF2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF279CF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2B579"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9179F2"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF83F279"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF279A7"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF28C79"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7988F2"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF79F2F1"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF79CAF2"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEDF279"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD379F2"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFACF279"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -777,31 +777,31 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
         <v>47</v>
       </c>
       <c r="M2" s="2"/>
-      <c r="N2" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="P2" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="Q2" s="2"/>
-      <c r="R2" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -821,27 +821,27 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="F3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
         <v>48</v>
       </c>
       <c r="M3" s="1"/>
-      <c r="N3" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="P3" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
@@ -872,22 +872,22 @@
         <v>27</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>24</v>
@@ -896,32 +896,28 @@
         <v>25</v>
       </c>
       <c r="N4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="T4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
@@ -938,66 +934,62 @@
         <v>0</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="F5" s="8" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="N5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="O5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" s="10" t="s">
+      <c r="T5" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="R5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="V5" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
@@ -1019,21 +1011,21 @@
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="7"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="4"/>
       <c r="Q6" s="8"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="8"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
@@ -1055,21 +1047,21 @@
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="4"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="8"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
@@ -1091,21 +1083,21 @@
       <c r="E8" s="7"/>
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="7"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="4"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="8"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
@@ -1127,21 +1119,21 @@
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="7"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="4"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="8"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
@@ -1163,21 +1155,21 @@
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="7"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="4"/>
       <c r="Q10" s="8"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="8"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
@@ -1212,8 +1204,8 @@
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
@@ -1229,60 +1221,62 @@
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="E12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="F12" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="12" t="s">
+      <c r="O12" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="R12" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="S12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="T12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="M12" s="1"/>
-      <c r="N12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="O12" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="P12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q12" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="R12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="S12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="T12" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="U12" s="14" t="s">
-        <v>37</v>
-      </c>
+      <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
@@ -1299,26 +1293,26 @@
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="16"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="10"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="15"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="18"/>
       <c r="O13" s="17"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="14"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
@@ -1335,26 +1329,26 @@
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="16"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="10"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="15"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="18"/>
       <c r="O14" s="17"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="14"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
@@ -1371,26 +1365,26 @@
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="16"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="15"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="18"/>
       <c r="O15" s="17"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="14"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
@@ -1407,26 +1401,26 @@
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="16"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="10"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="15"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="18"/>
       <c r="O16" s="17"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="14"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
@@ -1443,26 +1437,26 @@
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="16"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="10"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="15"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="18"/>
       <c r="O17" s="17"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="14"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
@@ -1498,8 +1492,8 @@
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
@@ -1516,50 +1510,44 @@
         <v>14</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>40</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="21" t="s">
+      <c r="F19" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="M19" s="1"/>
-      <c r="N19" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="O19" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="P19" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="S19" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="T19" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="L19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M19" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N19" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="O19" s="1"/>
+      <c r="P19" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q19" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
@@ -1579,23 +1567,23 @@
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="1"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="10"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="20"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
@@ -1615,23 +1603,23 @@
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
+      <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="1"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="10"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="20"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
@@ -1651,23 +1639,23 @@
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
+      <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="1"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="10"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="19"/>
-      <c r="T22" s="20"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
@@ -1687,23 +1675,23 @@
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
+      <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="1"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="10"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="21"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="21"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="20"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
@@ -1723,23 +1711,23 @@
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
+      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="1"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="10"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="21"/>
-      <c r="S24" s="19"/>
-      <c r="T24" s="20"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
@@ -1776,8 +1764,8 @@
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
@@ -1826,97 +1814,91 @@
       <c r="AF26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="90">
+  <mergeCells count="84">
     <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="C5:C10"/>
     <mergeCell ref="D5:D10"/>
     <mergeCell ref="E5:E10"/>
-    <mergeCell ref="F5:F10"/>
-    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:B17"/>
     <mergeCell ref="C12:C17"/>
     <mergeCell ref="D12:D17"/>
     <mergeCell ref="E12:E17"/>
-    <mergeCell ref="F12:F17"/>
-    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:B24"/>
     <mergeCell ref="C19:C24"/>
     <mergeCell ref="D19:D24"/>
     <mergeCell ref="E19:E24"/>
-    <mergeCell ref="F19:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F5:F10"/>
     <mergeCell ref="G5:G10"/>
     <mergeCell ref="H5:H10"/>
     <mergeCell ref="I5:I10"/>
-    <mergeCell ref="J5:J10"/>
-    <mergeCell ref="K5:K10"/>
-    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F12:F17"/>
     <mergeCell ref="G12:G17"/>
     <mergeCell ref="H12:H17"/>
     <mergeCell ref="I12:I17"/>
-    <mergeCell ref="J12:J17"/>
-    <mergeCell ref="K12:K17"/>
-    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F19:F24"/>
     <mergeCell ref="G19:G24"/>
     <mergeCell ref="H19:H24"/>
     <mergeCell ref="I19:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J5:J10"/>
+    <mergeCell ref="K5:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:J17"/>
+    <mergeCell ref="K12:K17"/>
+    <mergeCell ref="J18:K18"/>
     <mergeCell ref="J19:J24"/>
     <mergeCell ref="K19:K24"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="L3:O3"/>
     <mergeCell ref="L5:L10"/>
     <mergeCell ref="M5:M10"/>
-    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N5:N10"/>
+    <mergeCell ref="O5:O10"/>
+    <mergeCell ref="L11:O11"/>
     <mergeCell ref="L12:L17"/>
     <mergeCell ref="M12:M17"/>
-    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N12:N17"/>
+    <mergeCell ref="O12:O17"/>
+    <mergeCell ref="L18:O18"/>
     <mergeCell ref="L19:L24"/>
     <mergeCell ref="M19:M24"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="N5:N10"/>
-    <mergeCell ref="O5:O10"/>
+    <mergeCell ref="N19:N24"/>
+    <mergeCell ref="O19:O24"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="P3:T3"/>
     <mergeCell ref="P5:P10"/>
     <mergeCell ref="Q5:Q10"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="N12:N17"/>
-    <mergeCell ref="O12:O17"/>
-    <mergeCell ref="P12:P17"/>
-    <mergeCell ref="Q12:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N19:N24"/>
-    <mergeCell ref="O19:O24"/>
-    <mergeCell ref="P19:P24"/>
-    <mergeCell ref="Q19:Q24"/>
-    <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="R3:V3"/>
     <mergeCell ref="R5:R10"/>
     <mergeCell ref="S5:S10"/>
     <mergeCell ref="T5:T10"/>
-    <mergeCell ref="U5:U10"/>
-    <mergeCell ref="V5:V10"/>
-    <mergeCell ref="R11:V11"/>
+    <mergeCell ref="P11:T11"/>
+    <mergeCell ref="P12:P17"/>
+    <mergeCell ref="Q12:Q17"/>
     <mergeCell ref="R12:R17"/>
     <mergeCell ref="S12:S17"/>
     <mergeCell ref="T12:T17"/>
-    <mergeCell ref="U12:U17"/>
-    <mergeCell ref="V12:V17"/>
-    <mergeCell ref="R18:V18"/>
+    <mergeCell ref="P18:T18"/>
+    <mergeCell ref="P19:P24"/>
+    <mergeCell ref="Q19:Q24"/>
     <mergeCell ref="R19:R24"/>
     <mergeCell ref="S19:S24"/>
     <mergeCell ref="T19:T24"/>
-    <mergeCell ref="U19:U24"/>
-    <mergeCell ref="V19:V24"/>
-    <mergeCell ref="R25:V25"/>
-    <mergeCell ref="B1:V1"/>
+    <mergeCell ref="P25:T25"/>
+    <mergeCell ref="B1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>